<commit_message>
Added to Clang Format
</commit_message>
<xml_diff>
--- a/tools/instruction_type_mapping.xlsx
+++ b/tools/instruction_type_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="110" windowWidth="11900" windowHeight="3770"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Mapping" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -163,6 +164,12 @@
   </si>
   <si>
     <t>AR2</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -325,17 +332,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C257" totalsRowShown="0">
-  <autoFilter ref="A1:C257"/>
-  <sortState ref="A2:C257">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D257" totalsRowShown="0">
+  <autoFilter ref="A1:D257"/>
+  <sortState ref="A2:D257">
     <sortCondition ref="C1:C257"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" name="Dec Instr"/>
     <tableColumn id="2" name="Hex Instr" dataDxfId="8">
       <calculatedColumnFormula>DEC2HEX(A2,2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -628,19 +636,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C257"/>
+  <dimension ref="A1:D257"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242:B246"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -650,8 +658,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -662,8 +673,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -674,8 +688,11 @@
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>12</v>
       </c>
@@ -686,8 +703,11 @@
       <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>13</v>
       </c>
@@ -698,8 +718,11 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20</v>
       </c>
@@ -710,8 +733,11 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>21</v>
       </c>
@@ -722,8 +748,11 @@
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -734,8 +763,11 @@
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>29</v>
       </c>
@@ -746,8 +778,11 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>36</v>
       </c>
@@ -758,8 +793,11 @@
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>37</v>
       </c>
@@ -770,8 +808,11 @@
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>39</v>
       </c>
@@ -782,8 +823,11 @@
       <c r="C12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>44</v>
       </c>
@@ -794,8 +838,11 @@
       <c r="C13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>45</v>
       </c>
@@ -806,8 +853,11 @@
       <c r="C14" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>47</v>
       </c>
@@ -818,8 +868,11 @@
       <c r="C15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>52</v>
       </c>
@@ -830,8 +883,11 @@
       <c r="C16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>53</v>
       </c>
@@ -842,8 +898,11 @@
       <c r="C17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>55</v>
       </c>
@@ -854,8 +913,11 @@
       <c r="C18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>60</v>
       </c>
@@ -866,8 +928,11 @@
       <c r="C19" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>61</v>
       </c>
@@ -878,8 +943,11 @@
       <c r="C20" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>63</v>
       </c>
@@ -890,8 +958,11 @@
       <c r="C21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>128</v>
       </c>
@@ -902,8 +973,11 @@
       <c r="C22" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>129</v>
       </c>
@@ -914,8 +988,11 @@
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>130</v>
       </c>
@@ -926,8 +1003,11 @@
       <c r="C24" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>131</v>
       </c>
@@ -938,8 +1018,11 @@
       <c r="C25" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>132</v>
       </c>
@@ -950,8 +1033,11 @@
       <c r="C26" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>133</v>
       </c>
@@ -962,8 +1048,11 @@
       <c r="C27" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>134</v>
       </c>
@@ -974,8 +1063,11 @@
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>135</v>
       </c>
@@ -986,8 +1078,11 @@
       <c r="C29" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>136</v>
       </c>
@@ -998,8 +1093,11 @@
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>137</v>
       </c>
@@ -1010,8 +1108,11 @@
       <c r="C31" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>138</v>
       </c>
@@ -1022,8 +1123,11 @@
       <c r="C32" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>139</v>
       </c>
@@ -1034,8 +1138,11 @@
       <c r="C33" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>140</v>
       </c>
@@ -1046,8 +1153,11 @@
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>141</v>
       </c>
@@ -1058,8 +1168,11 @@
       <c r="C35" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>142</v>
       </c>
@@ -1070,8 +1183,11 @@
       <c r="C36" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>143</v>
       </c>
@@ -1082,8 +1198,11 @@
       <c r="C37" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>144</v>
       </c>
@@ -1094,8 +1213,11 @@
       <c r="C38" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>145</v>
       </c>
@@ -1106,8 +1228,11 @@
       <c r="C39" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>146</v>
       </c>
@@ -1118,8 +1243,11 @@
       <c r="C40" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>147</v>
       </c>
@@ -1130,8 +1258,11 @@
       <c r="C41" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>148</v>
       </c>
@@ -1142,8 +1273,11 @@
       <c r="C42" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>149</v>
       </c>
@@ -1154,8 +1288,11 @@
       <c r="C43" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>150</v>
       </c>
@@ -1166,8 +1303,11 @@
       <c r="C44" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>151</v>
       </c>
@@ -1178,8 +1318,11 @@
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>152</v>
       </c>
@@ -1190,8 +1333,11 @@
       <c r="C46" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>153</v>
       </c>
@@ -1202,8 +1348,11 @@
       <c r="C47" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>154</v>
       </c>
@@ -1214,8 +1363,11 @@
       <c r="C48" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>155</v>
       </c>
@@ -1226,8 +1378,11 @@
       <c r="C49" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>156</v>
       </c>
@@ -1238,8 +1393,11 @@
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>157</v>
       </c>
@@ -1250,8 +1408,11 @@
       <c r="C51" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>158</v>
       </c>
@@ -1262,8 +1423,11 @@
       <c r="C52" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>159</v>
       </c>
@@ -1274,8 +1438,11 @@
       <c r="C53" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>160</v>
       </c>
@@ -1286,8 +1453,11 @@
       <c r="C54" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>161</v>
       </c>
@@ -1298,8 +1468,11 @@
       <c r="C55" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>162</v>
       </c>
@@ -1310,8 +1483,11 @@
       <c r="C56" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>163</v>
       </c>
@@ -1322,8 +1498,11 @@
       <c r="C57" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>164</v>
       </c>
@@ -1334,8 +1513,11 @@
       <c r="C58" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>165</v>
       </c>
@@ -1346,8 +1528,11 @@
       <c r="C59" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>166</v>
       </c>
@@ -1358,8 +1543,11 @@
       <c r="C60" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>167</v>
       </c>
@@ -1370,8 +1558,11 @@
       <c r="C61" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>168</v>
       </c>
@@ -1382,8 +1573,11 @@
       <c r="C62" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>169</v>
       </c>
@@ -1394,8 +1588,11 @@
       <c r="C63" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>170</v>
       </c>
@@ -1406,8 +1603,11 @@
       <c r="C64" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>171</v>
       </c>
@@ -1418,8 +1618,11 @@
       <c r="C65" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>172</v>
       </c>
@@ -1430,8 +1633,11 @@
       <c r="C66" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>173</v>
       </c>
@@ -1442,8 +1648,11 @@
       <c r="C67" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>174</v>
       </c>
@@ -1454,8 +1663,11 @@
       <c r="C68" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>175</v>
       </c>
@@ -1466,8 +1678,11 @@
       <c r="C69" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>176</v>
       </c>
@@ -1478,8 +1693,11 @@
       <c r="C70" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>177</v>
       </c>
@@ -1490,8 +1708,11 @@
       <c r="C71" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>178</v>
       </c>
@@ -1502,8 +1723,11 @@
       <c r="C72" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>179</v>
       </c>
@@ -1514,8 +1738,11 @@
       <c r="C73" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>180</v>
       </c>
@@ -1526,8 +1753,11 @@
       <c r="C74" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>181</v>
       </c>
@@ -1538,8 +1768,11 @@
       <c r="C75" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>182</v>
       </c>
@@ -1550,8 +1783,11 @@
       <c r="C76" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>183</v>
       </c>
@@ -1562,8 +1798,11 @@
       <c r="C77" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>184</v>
       </c>
@@ -1574,8 +1813,11 @@
       <c r="C78" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>185</v>
       </c>
@@ -1586,8 +1828,11 @@
       <c r="C79" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>186</v>
       </c>
@@ -1598,8 +1843,11 @@
       <c r="C80" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>187</v>
       </c>
@@ -1610,8 +1858,11 @@
       <c r="C81" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>188</v>
       </c>
@@ -1622,8 +1873,11 @@
       <c r="C82" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>189</v>
       </c>
@@ -1634,8 +1888,11 @@
       <c r="C83" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>190</v>
       </c>
@@ -1646,8 +1903,11 @@
       <c r="C84" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>191</v>
       </c>
@@ -1658,8 +1918,11 @@
       <c r="C85" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>198</v>
       </c>
@@ -1670,8 +1933,11 @@
       <c r="C86" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>206</v>
       </c>
@@ -1682,8 +1948,11 @@
       <c r="C87" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>214</v>
       </c>
@@ -1694,8 +1963,11 @@
       <c r="C88" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>222</v>
       </c>
@@ -1706,8 +1978,11 @@
       <c r="C89" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>230</v>
       </c>
@@ -1718,8 +1993,11 @@
       <c r="C90" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>238</v>
       </c>
@@ -1730,8 +2008,11 @@
       <c r="C91" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>246</v>
       </c>
@@ -1742,8 +2023,11 @@
       <c r="C92" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>254</v>
       </c>
@@ -1754,8 +2038,11 @@
       <c r="C93" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>3</v>
       </c>
@@ -1766,8 +2053,11 @@
       <c r="C94" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>9</v>
       </c>
@@ -1778,8 +2068,11 @@
       <c r="C95" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>11</v>
       </c>
@@ -1790,8 +2083,11 @@
       <c r="C96" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>19</v>
       </c>
@@ -1802,8 +2098,11 @@
       <c r="C97" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>25</v>
       </c>
@@ -1814,8 +2113,11 @@
       <c r="C98" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>27</v>
       </c>
@@ -1826,8 +2128,11 @@
       <c r="C99" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>35</v>
       </c>
@@ -1838,8 +2143,11 @@
       <c r="C100" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>41</v>
       </c>
@@ -1850,8 +2158,11 @@
       <c r="C101" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>43</v>
       </c>
@@ -1862,8 +2173,11 @@
       <c r="C102" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>51</v>
       </c>
@@ -1874,8 +2188,11 @@
       <c r="C103" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>57</v>
       </c>
@@ -1886,8 +2203,11 @@
       <c r="C104" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>59</v>
       </c>
@@ -1898,8 +2218,11 @@
       <c r="C105" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>232</v>
       </c>
@@ -1910,8 +2233,11 @@
       <c r="C106" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>24</v>
       </c>
@@ -1923,7 +2249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>32</v>
       </c>
@@ -1934,8 +2260,9 @@
       <c r="C108" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>40</v>
       </c>
@@ -1947,7 +2274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>48</v>
       </c>
@@ -1958,8 +2285,9 @@
       <c r="C110" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>56</v>
       </c>
@@ -1971,7 +2299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>192</v>
       </c>
@@ -1982,8 +2310,9 @@
       <c r="C112" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>194</v>
       </c>
@@ -1995,7 +2324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>195</v>
       </c>
@@ -2007,7 +2336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>196</v>
       </c>
@@ -2019,7 +2348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>199</v>
       </c>
@@ -2031,7 +2360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>200</v>
       </c>
@@ -2043,7 +2372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>201</v>
       </c>
@@ -2055,7 +2384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>202</v>
       </c>
@@ -2067,7 +2396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>204</v>
       </c>
@@ -2079,7 +2408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>205</v>
       </c>
@@ -2091,7 +2420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>207</v>
       </c>
@@ -2103,7 +2432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>208</v>
       </c>
@@ -2114,8 +2443,9 @@
       <c r="C123" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>210</v>
       </c>
@@ -2127,7 +2457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>212</v>
       </c>
@@ -2139,7 +2469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>215</v>
       </c>
@@ -2151,7 +2481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>216</v>
       </c>
@@ -2163,7 +2493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>217</v>
       </c>
@@ -2175,7 +2505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>218</v>
       </c>
@@ -2187,7 +2517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>220</v>
       </c>
@@ -2199,7 +2529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>223</v>
       </c>
@@ -2211,7 +2541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>231</v>
       </c>
@@ -2223,7 +2553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>233</v>
       </c>
@@ -2235,7 +2565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>239</v>
       </c>
@@ -2247,7 +2577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>247</v>
       </c>
@@ -2259,7 +2589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>255</v>
       </c>
@@ -2271,7 +2601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2</v>
       </c>
@@ -2283,7 +2613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>6</v>
       </c>
@@ -2295,7 +2625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>10</v>
       </c>
@@ -2307,7 +2637,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>14</v>
       </c>
@@ -2319,7 +2649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>18</v>
       </c>
@@ -2331,7 +2661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>22</v>
       </c>
@@ -2343,7 +2673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>26</v>
       </c>
@@ -2355,7 +2685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>30</v>
       </c>
@@ -2367,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>34</v>
       </c>
@@ -2379,7 +2709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>38</v>
       </c>
@@ -2391,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>42</v>
       </c>
@@ -2403,7 +2733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>46</v>
       </c>
@@ -2415,7 +2745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>50</v>
       </c>
@@ -2427,7 +2757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>54</v>
       </c>
@@ -2439,7 +2769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>58</v>
       </c>
@@ -2451,7 +2781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>62</v>
       </c>
@@ -2463,7 +2793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>64</v>
       </c>
@@ -2474,8 +2804,9 @@
       <c r="C153" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>65</v>
       </c>
@@ -2487,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>66</v>
       </c>
@@ -2499,7 +2830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="3">
         <v>67</v>
       </c>
@@ -2511,7 +2842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>68</v>
       </c>
@@ -2523,7 +2854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>69</v>
       </c>
@@ -2535,7 +2866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>70</v>
       </c>
@@ -2547,7 +2878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>71</v>
       </c>
@@ -2559,7 +2890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>72</v>
       </c>
@@ -2571,7 +2902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>73</v>
       </c>
@@ -2583,7 +2914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>74</v>
       </c>
@@ -2595,7 +2926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="3">
         <v>75</v>
       </c>
@@ -2607,7 +2938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>76</v>
       </c>
@@ -2619,7 +2950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>77</v>
       </c>
@@ -2631,7 +2962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>78</v>
       </c>
@@ -2643,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>79</v>
       </c>
@@ -2655,7 +2986,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="3">
         <v>80</v>
       </c>
@@ -2666,8 +2997,9 @@
       <c r="C169" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>81</v>
       </c>
@@ -2679,7 +3011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>82</v>
       </c>
@@ -2691,7 +3023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" s="3">
         <v>83</v>
       </c>
@@ -2703,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>84</v>
       </c>
@@ -2715,7 +3047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>85</v>
       </c>
@@ -2727,7 +3059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>86</v>
       </c>
@@ -2739,7 +3071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>87</v>
       </c>
@@ -2751,7 +3083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>88</v>
       </c>
@@ -2763,7 +3095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>89</v>
       </c>
@@ -2775,7 +3107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" s="3">
         <v>90</v>
       </c>
@@ -2787,7 +3119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>91</v>
       </c>
@@ -2799,7 +3131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>92</v>
       </c>
@@ -2811,7 +3143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>93</v>
       </c>
@@ -2823,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>94</v>
       </c>
@@ -2835,7 +3167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>95</v>
       </c>
@@ -2847,7 +3179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="3">
         <v>96</v>
       </c>
@@ -2858,8 +3190,9 @@
       <c r="C185" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>97</v>
       </c>
@@ -2871,7 +3204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>98</v>
       </c>
@@ -2883,7 +3216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" s="3">
         <v>99</v>
       </c>
@@ -2895,7 +3228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>100</v>
       </c>
@@ -2907,7 +3240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>101</v>
       </c>
@@ -2919,7 +3252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>102</v>
       </c>
@@ -2931,7 +3264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>103</v>
       </c>
@@ -2943,7 +3276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>104</v>
       </c>
@@ -2955,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>105</v>
       </c>
@@ -2967,7 +3300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>106</v>
       </c>
@@ -2979,7 +3312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>107</v>
       </c>
@@ -2991,7 +3324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>108</v>
       </c>
@@ -3003,7 +3336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>109</v>
       </c>
@@ -3015,7 +3348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>110</v>
       </c>
@@ -3027,7 +3360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>111</v>
       </c>
@@ -3039,7 +3372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="3">
         <v>112</v>
       </c>
@@ -3050,8 +3383,9 @@
       <c r="C201" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>113</v>
       </c>
@@ -3063,7 +3397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>114</v>
       </c>
@@ -3075,7 +3409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" s="3">
         <v>115</v>
       </c>
@@ -3087,7 +3421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>116</v>
       </c>
@@ -3099,7 +3433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>117</v>
       </c>
@@ -3111,7 +3445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>119</v>
       </c>
@@ -3123,7 +3457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" s="3">
         <v>120</v>
       </c>
@@ -3135,7 +3469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>121</v>
       </c>
@@ -3147,7 +3481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>122</v>
       </c>
@@ -3159,7 +3493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>123</v>
       </c>
@@ -3171,7 +3505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>124</v>
       </c>
@@ -3183,7 +3517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>125</v>
       </c>
@@ -3195,7 +3529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>126</v>
       </c>
@@ -3207,7 +3541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>127</v>
       </c>
@@ -3219,7 +3553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" s="3">
         <v>224</v>
       </c>
@@ -3230,8 +3564,9 @@
       <c r="C216" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>226</v>
       </c>
@@ -3243,7 +3578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>234</v>
       </c>
@@ -3255,7 +3590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" s="3">
         <v>240</v>
       </c>
@@ -3266,8 +3601,9 @@
       <c r="C219" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>242</v>
       </c>
@@ -3279,7 +3615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>250</v>
       </c>
@@ -3291,7 +3627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>1</v>
       </c>
@@ -3303,7 +3639,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>8</v>
       </c>
@@ -3315,7 +3651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>17</v>
       </c>
@@ -3327,7 +3663,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>33</v>
       </c>
@@ -3339,7 +3675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="226" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A226" s="1">
         <v>49</v>
       </c>
@@ -3351,7 +3687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>193</v>
       </c>
@@ -3363,7 +3699,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>197</v>
       </c>
@@ -3375,7 +3711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>209</v>
       </c>
@@ -3387,7 +3723,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>213</v>
       </c>
@@ -3399,7 +3735,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A231" s="3">
         <v>225</v>
       </c>
@@ -3411,7 +3747,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>229</v>
       </c>
@@ -3423,7 +3759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>241</v>
       </c>
@@ -3435,7 +3771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>245</v>
       </c>
@@ -3447,7 +3783,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>248</v>
       </c>
@@ -3459,7 +3795,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>249</v>
       </c>
@@ -3471,7 +3807,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>7</v>
       </c>
@@ -3483,7 +3819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>15</v>
       </c>
@@ -3495,7 +3831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>23</v>
       </c>
@@ -3507,7 +3843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>31</v>
       </c>
@@ -3519,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" s="3">
         <v>203</v>
       </c>
@@ -3531,7 +3867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A242" s="1">
         <v>0</v>
       </c>
@@ -3543,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A243" s="3">
         <v>16</v>
       </c>
@@ -3554,8 +3890,9 @@
       <c r="C243" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>118</v>
       </c>
@@ -3567,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>243</v>
       </c>
@@ -3579,7 +3916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>251</v>
       </c>
@@ -3591,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>211</v>
       </c>
@@ -3600,7 +3937,7 @@
         <v>D3</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>219</v>
       </c>
@@ -3610,7 +3947,7 @@
       </c>
       <c r="C248" s="3"/>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>221</v>
       </c>
@@ -3619,7 +3956,7 @@
         <v>DD</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>227</v>
       </c>
@@ -3628,7 +3965,7 @@
         <v>E3</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>228</v>
       </c>
@@ -3637,7 +3974,7 @@
         <v>E4</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>235</v>
       </c>
@@ -3646,7 +3983,7 @@
         <v>EB</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>236</v>
       </c>
@@ -3655,7 +3992,7 @@
         <v>EC</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>237</v>
       </c>
@@ -3664,7 +4001,7 @@
         <v>ED</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>244</v>
       </c>
@@ -3673,7 +4010,7 @@
         <v>F4</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>252</v>
       </c>
@@ -3682,7 +4019,7 @@
         <v>FC</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>253</v>
       </c>
@@ -3707,9 +4044,9 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -3807,7 +4144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3931,7 +4268,7 @@
         <v>15</v>
       </c>
       <c r="AF2">
-        <f t="shared" ref="AF2:AG2" si="2">AE2+1</f>
+        <f t="shared" ref="AF2:AG17" si="2">AE2+1</f>
         <v>16</v>
       </c>
       <c r="AG2">
@@ -3939,7 +4276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -4064,15 +4401,15 @@
         <v>31</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AG3" si="5">AE3+1</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="AG3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4141,7 +4478,7 @@
         <v>AR</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R17" si="6">R3+16</f>
+        <f t="shared" ref="R4:R17" si="5">R3+16</f>
         <v>34</v>
       </c>
       <c r="S4">
@@ -4197,15 +4534,15 @@
         <v>47</v>
       </c>
       <c r="AF4">
-        <f t="shared" ref="AF4:AG4" si="7">AE4+1</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="7"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -4274,7 +4611,7 @@
         <v>AR</v>
       </c>
       <c r="R5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="S5">
@@ -4330,15 +4667,15 @@
         <v>63</v>
       </c>
       <c r="AF5">
-        <f t="shared" ref="AF5:AG5" si="8">AE5+1</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -4407,7 +4744,7 @@
         <v>AR</v>
       </c>
       <c r="R6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="S6">
@@ -4463,15 +4800,15 @@
         <v>79</v>
       </c>
       <c r="AF6">
-        <f t="shared" ref="AF6:AG6" si="9">AE6+1</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -4540,7 +4877,7 @@
         <v>AR2</v>
       </c>
       <c r="R7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>82</v>
       </c>
       <c r="S7">
@@ -4596,15 +4933,15 @@
         <v>95</v>
       </c>
       <c r="AF7">
-        <f t="shared" ref="AF7:AG7" si="10">AE7+1</f>
+        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -4673,7 +5010,7 @@
         <v>FL</v>
       </c>
       <c r="R8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>98</v>
       </c>
       <c r="S8">
@@ -4729,15 +5066,15 @@
         <v>111</v>
       </c>
       <c r="AF8">
-        <f t="shared" ref="AF8:AG8" si="11">AE8+1</f>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -4806,7 +5143,7 @@
         <v>FL</v>
       </c>
       <c r="R9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>114</v>
       </c>
       <c r="S9">
@@ -4862,15 +5199,15 @@
         <v>127</v>
       </c>
       <c r="AF9">
-        <f t="shared" ref="AF9:AG9" si="12">AE9+1</f>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -4939,7 +5276,7 @@
         <v>LD</v>
       </c>
       <c r="R10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
       <c r="S10">
@@ -4995,15 +5332,15 @@
         <v>143</v>
       </c>
       <c r="AF10">
-        <f t="shared" ref="AF10:AG10" si="13">AE10+1</f>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -5072,7 +5409,7 @@
         <v>LD</v>
       </c>
       <c r="R11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>146</v>
       </c>
       <c r="S11">
@@ -5128,15 +5465,15 @@
         <v>159</v>
       </c>
       <c r="AF11">
-        <f t="shared" ref="AF11:AG11" si="14">AE11+1</f>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="2"/>
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -5205,7 +5542,7 @@
         <v>LD</v>
       </c>
       <c r="R12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>162</v>
       </c>
       <c r="S12">
@@ -5261,15 +5598,15 @@
         <v>175</v>
       </c>
       <c r="AF12">
-        <f t="shared" ref="AF12:AG12" si="15">AE12+1</f>
+        <f t="shared" si="2"/>
         <v>176</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -5338,7 +5675,7 @@
         <v>LD</v>
       </c>
       <c r="R13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="S13">
@@ -5394,15 +5731,15 @@
         <v>191</v>
       </c>
       <c r="AF13">
-        <f t="shared" ref="AF13:AG13" si="16">AE13+1</f>
+        <f t="shared" si="2"/>
         <v>192</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="2"/>
         <v>193</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -5471,7 +5808,7 @@
         <v>LD</v>
       </c>
       <c r="R14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>194</v>
       </c>
       <c r="S14">
@@ -5527,15 +5864,15 @@
         <v>207</v>
       </c>
       <c r="AF14">
-        <f t="shared" ref="AF14:AG14" si="17">AE14+1</f>
+        <f t="shared" si="2"/>
         <v>208</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -5604,7 +5941,7 @@
         <v>LD2</v>
       </c>
       <c r="R15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
       <c r="S15">
@@ -5660,15 +5997,15 @@
         <v>223</v>
       </c>
       <c r="AF15">
-        <f t="shared" ref="AF15:AG15" si="18">AE15+1</f>
+        <f t="shared" si="2"/>
         <v>224</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -5737,7 +6074,7 @@
         <v>LG</v>
       </c>
       <c r="R16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>226</v>
       </c>
       <c r="S16">
@@ -5793,15 +6130,15 @@
         <v>239</v>
       </c>
       <c r="AF16">
-        <f t="shared" ref="AF16:AG16" si="19">AE16+1</f>
+        <f t="shared" si="2"/>
         <v>240</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="2"/>
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -5870,7 +6207,7 @@
         <v>0</v>
       </c>
       <c r="R17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>242</v>
       </c>
       <c r="S17">
@@ -5926,11 +6263,11 @@
         <v>255</v>
       </c>
       <c r="AF17">
-        <f t="shared" ref="AF17:AG17" si="20">AE17+1</f>
+        <f t="shared" si="2"/>
         <v>256</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="20"/>
+        <f t="shared" si="2"/>
         <v>257</v>
       </c>
     </row>
@@ -5970,9 +6307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>